<commit_message>
penyesuaian tampilan dashboard, migration database terbaru dan tampilan blade
</commit_message>
<xml_diff>
--- a/public/template/template_penetapan.xlsx
+++ b/public/template/template_penetapan.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/FACHREZA/PROJEK/web_penagihan 4/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/fahrezatualeka/PROJEK/smantap/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E293CC19-704C-104F-A524-3C98114C381A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA472D9-7791-BE4D-B08D-4F1437EBA70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{21DFCAA3-0EED-EB47-BDF0-C28D624CC039}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,25 +35,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>npwpd</t>
   </si>
   <si>
-    <t>jumlah_penetapan</t>
+    <t>jumlah_penagihan</t>
+  </si>
+  <si>
+    <t>P.2.0021240.03.003</t>
+  </si>
+  <si>
+    <t>P.2.0021556.01.011</t>
+  </si>
+  <si>
+    <t>P.2.0001580.04.009.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,8 +97,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,23 +415,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3737DEF9-6009-8E45-B158-4A1AE3890014}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>400000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
penghapusan tombol edit dan hapus, penambahan pembagian zonasi di datawajibpajak
</commit_message>
<xml_diff>
--- a/public/template/template_penetapan.xlsx
+++ b/public/template/template_penetapan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/fahrezatualeka/PROJEK/smantap/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA472D9-7791-BE4D-B08D-4F1437EBA70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{56FCA49E-216C-164C-B716-3FED6F2F9C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{21DFCAA3-0EED-EB47-BDF0-C28D624CC039}"/>
   </bookViews>
@@ -35,21 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>npwpd</t>
   </si>
   <si>
     <t>jumlah_penagihan</t>
-  </si>
-  <si>
-    <t>P.2.0021240.03.003</t>
-  </si>
-  <si>
-    <t>P.2.0021556.01.011</t>
-  </si>
-  <si>
-    <t>P.2.0001580.04.009.</t>
   </si>
 </sst>
 </file>
@@ -73,7 +64,7 @@
     <font>
       <sz val="14"/>
       <color rgb="FF333333"/>
-      <name val="Helvetica Neue"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -418,16 +409,17 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,29 +427,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>120000</v>
-      </c>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>2000</v>
-      </c>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>400000</v>
-      </c>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>